<commit_message>
Planilla de ejemplo finalizada
</commit_message>
<xml_diff>
--- a/PlanillaBodega.xlsx
+++ b/PlanillaBodega.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\Documents\GitHub\beetrackManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B710CE9-2C06-4D0C-9CB8-3FE95C7A4133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6CEDAE-530C-48A4-85C1-2612886FBB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43B46EBB-21CF-4422-BC23-C7117958AA10}"/>
   </bookViews>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719CDBC3-2C9D-4FD4-A760-5075530AFB36}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cambiada opción "Sin documento" para coincidir con la planilla de despachos
</commit_message>
<xml_diff>
--- a/PlanillaBodega.xlsx
+++ b/PlanillaBodega.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\Documents\GitHub\beetrackManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6CEDAE-530C-48A4-85C1-2612886FBB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B776723-DA0B-4FE6-9BE8-7F4C6E6438C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43B46EBB-21CF-4422-BC23-C7117958AA10}"/>
+    <workbookView xWindow="4065" yWindow="4050" windowWidth="21600" windowHeight="11295" xr2:uid="{43B46EBB-21CF-4422-BC23-C7117958AA10}"/>
   </bookViews>
   <sheets>
     <sheet name="Control de ingresos" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>Otro</t>
   </si>
   <si>
-    <t>Sin documentos</t>
-  </si>
-  <si>
     <t>Guía de despacho</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>N de Bultos</t>
+  </si>
+  <si>
+    <t>Sin documento</t>
   </si>
 </sst>
 </file>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719CDBC3-2C9D-4FD4-A760-5075530AFB36}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,13 +792,13 @@
   <sheetData>
     <row r="1" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>1</v>
@@ -843,10 +843,10 @@
         <v>14</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T1" s="7" t="s">
         <v>15</v>
@@ -859,46 +859,46 @@
     </row>
     <row r="2" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="11">
         <v>495</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="M2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N2" s="12">
         <v>44469.416666666664</v>
       </c>
       <c r="O2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="R2" s="9">
         <v>8</v>
@@ -907,45 +907,45 @@
         <v>40</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="F3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="M3" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N3" s="13">
         <v>44470.416666666664</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R3" s="9">
         <v>1</v>
@@ -954,49 +954,49 @@
         <v>8</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="M4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N4" s="13"/>
       <c r="O4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="R4" s="9">
         <v>8</v>
@@ -1005,10 +1005,10 @@
         <v>48</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,19 +1153,19 @@
         <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1173,36 +1173,36 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1210,10 +1210,10 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1223,7 +1223,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>